<commit_message>
Import dosyasına hedefler eklendi.
</commit_message>
<xml_diff>
--- a/Şablonlar/Ek Tablolar.xlsx
+++ b/Şablonlar/Ek Tablolar.xlsx
@@ -5,26 +5,55 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serdar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSRepo\Projects\SirketBI\trunk\Şablonlar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="0" windowWidth="27180" windowHeight="13020"/>
+    <workbookView xWindow="8100" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="TekBrans" sheetId="1" r:id="rId1"/>
+    <sheet name="Hedefler" sheetId="2" r:id="rId2"/>
+    <sheet name="SirketTanimliUrun" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hedefler!$A$1:$E$1</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Teknik Branş</t>
   </si>
   <si>
     <t>Özel Branş Grubu</t>
+  </si>
+  <si>
+    <t>BÖLGE</t>
+  </si>
+  <si>
+    <t>BRANS</t>
+  </si>
+  <si>
+    <t>YIL</t>
+  </si>
+  <si>
+    <t>AY</t>
+  </si>
+  <si>
+    <t>HEDEF ÜRETİM</t>
+  </si>
+  <si>
+    <t>UrunKodu</t>
+  </si>
+  <si>
+    <t>UrunGrubu</t>
+  </si>
+  <si>
+    <t>UrunAdi</t>
   </si>
 </sst>
 </file>
@@ -346,7 +375,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -367,4 +396,70 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD121"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Import dosyalarında excelden alınacak şekilde ZeyilSirketTanimli tablosu eklendi.
</commit_message>
<xml_diff>
--- a/Şablonlar/Ek Tablolar.xlsx
+++ b/Şablonlar/Ek Tablolar.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSRepo\Projects\SirketBI\trunk\Şablonlar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Power BI Raporlar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="9720" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="TekBrans" sheetId="1" r:id="rId1"/>
     <sheet name="Hedefler" sheetId="2" r:id="rId2"/>
     <sheet name="SirketTanimliUrun" sheetId="3" r:id="rId3"/>
+    <sheet name="Zeyiller" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hedefler!$A$1:$E$1</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Teknik Branş</t>
   </si>
@@ -54,6 +55,9 @@
   </si>
   <si>
     <t>UrunAdi</t>
+  </si>
+  <si>
+    <t>ZeyilKod</t>
   </si>
 </sst>
 </file>
@@ -380,8 +384,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -408,8 +412,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="44.25" customWidth="1"/>
+    <col min="5" max="5" width="13.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -439,13 +443,13 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD121"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -462,4 +466,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>